<commit_message>
Work on the Arduino Watch and Final Report
</commit_message>
<xml_diff>
--- a/Documents/Arduino Watch Components.xlsx
+++ b/Documents/Arduino Watch Components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT-Digital-Systems-Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732CAC49-E708-4499-9C2C-8A315F2B35AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{732CAC49-E708-4499-9C2C-8A315F2B35AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47AC9455-0C26-4965-BB52-572173E8A17E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{F7B5C95A-D014-4766-8A4F-EFF1A2859BC0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F7B5C95A-D014-4766-8A4F-EFF1A2859BC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Product</t>
   </si>
@@ -47,9 +47,6 @@
     <t>SKU</t>
   </si>
   <si>
-    <t xml:space="preserve">Quanitity </t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>TinyScreen+ (Processor, OLED &amp; USB in one)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity </t>
   </si>
 </sst>
 </file>
@@ -168,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -191,11 +191,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -204,19 +241,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -237,9 +280,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -277,7 +320,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -383,7 +426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -525,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -536,7 +579,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,203 +599,196 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>9</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>45600</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>10</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>45600</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>4</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>45600</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>15</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>45600</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>8.4499999999999993</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>45311</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>12</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>45314</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>15</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>45314</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>45314</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>5</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>45314</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>10</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>45314</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="7">
-        <f>SUM(C11:C11)</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="A12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9">
         <f>SUM(D2:D11)</f>
         <v>93.45</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="E12" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E11" xr:uid="{691627D9-55B6-474E-A8A2-FCC413AC4745}">
@@ -760,6 +796,10 @@
       <sortCondition descending="1" ref="E1:E11"/>
     </sortState>
   </autoFilter>
+  <mergeCells count="2">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:E12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>